<commit_message>
2nd sensor measurement analysis
</commit_message>
<xml_diff>
--- a/New measurements 20200108/2nd Sensor/2nd_sensor_sourcevoltagevariation.xlsx
+++ b/New measurements 20200108/2nd Sensor/2nd_sensor_sourcevoltagevariation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rijk\Documents\MEP\MEP_control_software\New measurements 20200108\2nd Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{349B559C-C713-44D0-AF63-02CEFBD20B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCE998E-5083-4095-9D53-CB22575FEBC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C83BDEB2-042E-446D-B18D-70EA549B34D7}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +508,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="1">
-        <v>80000</v>
+        <v>27099700000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -518,8 +518,8 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1">
-        <v>0.43</v>
+      <c r="I4">
+        <v>1.53691</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -536,8 +536,8 @@
         <v>55.404449999999997</v>
       </c>
       <c r="E5" s="1">
-        <f>LN((Table1[[#This Row],[Mean R]]-I5)/I3)/LN(I4)</f>
-        <v>-0.68523730056845777</v>
+        <f>$I$3*Table1[[#This Row],[Mean R]]^-$I$4 + $I$5</f>
+        <v>336.23320005037971</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -545,8 +545,8 @@
       <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1">
-        <v>-3600</v>
+      <c r="I5">
+        <v>-1.36972</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -562,6 +562,10 @@
       <c r="D6" s="1">
         <v>316.65480000000002</v>
       </c>
+      <c r="E6" s="1">
+        <f>$I$3*Table1[[#This Row],[Mean R]]^-$I$4 + $I$5</f>
+        <v>350.87029083172831</v>
+      </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
@@ -578,6 +582,10 @@
       </c>
       <c r="D7" s="1">
         <v>335.9194</v>
+      </c>
+      <c r="E7" s="1">
+        <f>$I$3*Table1[[#This Row],[Mean R]]^-$I$4 + $I$5</f>
+        <v>343.34592959776711</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>

</xml_diff>